<commit_message>
updated prediction and seasonality
</commit_message>
<xml_diff>
--- a/seasonality_chacla.xlsx
+++ b/seasonality_chacla.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RevPAR" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="37">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t xml:space="preserve">Inmaculada Concepción</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Batalla de Ayacucho</t>
   </si>
   <si>
     <t xml:space="preserve">Navidad</t>
@@ -247,11 +244,11 @@
   </sheetPr>
   <dimension ref="A1:C366"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A331" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A365" activeCellId="0" sqref="A365"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4295,13 +4292,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -4345,15 +4342,15 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>44539</v>
+        <v>44555</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>44555</v>
+      <c r="A7" s="3" t="n">
+        <v>44562</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
@@ -4361,15 +4358,15 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
-        <v>44562</v>
+        <v>44665</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>44665</v>
+      <c r="A9" s="1" t="n">
+        <v>44666</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>18</v>
@@ -4377,7 +4374,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>44666</v>
+        <v>44668</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
@@ -4385,7 +4382,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>44668</v>
+        <v>44682</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>20</v>
@@ -4393,7 +4390,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>44682</v>
+        <v>44741</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
@@ -4401,7 +4398,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>44741</v>
+        <v>44770</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>22</v>
@@ -4409,23 +4406,155 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>44770</v>
+        <v>44771</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>44771</v>
+        <v>44803</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="1" t="n">
+        <v>44842</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>44866</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>44903</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>44920</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="n">
+        <v>45022</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="n">
+        <v>45023</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="n">
+        <v>45025</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>45106</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>45135</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>45136</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>45168</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>45207</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>45268</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>45285</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4449,19 +4578,19 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>18</v>
@@ -4469,7 +4598,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>15</v>
@@ -4477,7 +4606,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>16</v>
@@ -4485,7 +4614,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>19</v>
@@ -4493,7 +4622,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>44</v>
@@ -4501,7 +4630,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>15</v>
@@ -4509,7 +4638,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>16</v>
@@ -4517,7 +4646,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>11</v>
@@ -4525,7 +4654,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>19</v>
@@ -4533,7 +4662,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>14</v>
@@ -4541,7 +4670,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>15</v>
@@ -4549,7 +4678,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>90</v>

</xml_diff>